<commit_message>
📝 Updated documentation by using `pandoc`
</commit_message>
<xml_diff>
--- a/data/output/combined-kpis.xlsx
+++ b/data/output/combined-kpis.xlsx
@@ -514,7 +514,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[(737, 50), (1291, 48), (1094, 48), (1171, 47), (659, 47), (1289, 47), (646, 46), (1324, 44), (1090, 44), (984, 43)]</t>
+          <t>[(737, 50), (1094, 48), (1291, 48), (659, 47), (1171, 47), (1289, 47), (646, 46), (1324, 44), (1090, 44), (984, 43)]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -562,7 +562,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[(1291, 37), (1107, 37), (1077, 36), (990, 35), (1046, 33), (736, 32), (780, 31), (1289, 29), (1139, 29), (822, 29)]</t>
+          <t>[(1291, 37), (1107, 37), (1077, 36), (990, 35), (1046, 33), (736, 32), (780, 31), (1139, 29), (1289, 29), (822, 29)]</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -610,7 +610,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>[(1098, 72), (883, 64), (1302, 61), (660, 61), (1086, 60), (1081, 59), (1096, 59), (771, 59), (773, 59), (769, 58)]</t>
+          <t>[(1098, 72), (883, 64), (1302, 61), (660, 61), (1086, 60), (771, 59), (1096, 59), (1081, 59), (773, 59), (769, 58)]</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">

</xml_diff>